<commit_message>
including multiple dose time-series, but cutting them off where it's possible to get a clean, first dose time-series
</commit_message>
<xml_diff>
--- a/Data/Systematic Review Results & Data Extraction.xlsx
+++ b/Data/Systematic Review Results & Data Extraction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cw1716\Documents\Q_Drive_Copy\Loa_Loa\Drug Efficacy Modelling\Albendazole Modelling\Albendazole PK Paper\albendazole_pk\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D616D507-22B2-43FD-9389-F25569ADFA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8224015-6C36-4730-9DED-08C5869F9DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="953" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9765" yWindow="3600" windowWidth="21600" windowHeight="11385" tabRatio="953" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall_Data" sheetId="26" r:id="rId1"/>
@@ -1647,8 +1647,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1689,11 +1687,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1702,6 +1696,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1986,7 +1986,7 @@
   <dimension ref="A1:XEZ53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2017,1700 +2017,1700 @@
       <c r="A2" s="11"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="53" t="s">
         <v>448</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="46" t="s">
+      <c r="G3" s="54"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="51"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="52"/>
-      <c r="U3" s="58" t="s">
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="45"/>
+      <c r="S3" s="45"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="52" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="26" t="s">
         <v>447</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="18" t="s">
         <v>313</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="M4" s="18" t="s">
         <v>323</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="N4" s="18" t="s">
         <v>346</v>
       </c>
-      <c r="O4" s="20" t="s">
+      <c r="O4" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="P4" s="20" t="s">
+      <c r="P4" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="Q4" s="20" t="s">
+      <c r="Q4" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="R4" s="20" t="s">
+      <c r="R4" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="S4" s="20" t="s">
+      <c r="S4" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="T4" s="29" t="s">
+      <c r="T4" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="U4" s="55"/>
+      <c r="U4" s="49"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="30">
+      <c r="A5" s="28">
         <v>2</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="29">
         <v>2003</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="28">
         <v>2</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="21">
         <v>0</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="21">
         <v>1</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="37">
-        <v>400</v>
-      </c>
-      <c r="J5" s="23" t="s">
+      <c r="I5" s="35">
+        <v>400</v>
+      </c>
+      <c r="J5" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K5" s="23" t="s">
+      <c r="K5" s="21" t="s">
         <v>321</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="L5" s="21" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="23" t="s">
+      <c r="M5" s="21" t="s">
         <v>324</v>
       </c>
-      <c r="N5" s="23" t="s">
+      <c r="N5" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="O5" s="38" t="s">
+      <c r="O5" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="23">
+      <c r="P5" s="21">
         <v>1</v>
       </c>
-      <c r="Q5" s="23" t="s">
+      <c r="Q5" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="R5" s="23" t="s">
+      <c r="R5" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S5" s="23" t="s">
+      <c r="S5" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="T5" s="31" t="s">
+      <c r="T5" s="29" t="s">
         <v>302</v>
       </c>
-      <c r="U5" s="55" t="s">
+      <c r="U5" s="49" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="30">
+      <c r="A6" s="28">
         <v>3</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="29">
         <v>2004</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="28">
         <v>2</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="21">
         <v>0</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="21">
         <v>1</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="37">
-        <v>400</v>
-      </c>
-      <c r="J6" s="23" t="s">
+      <c r="I6" s="35">
+        <v>400</v>
+      </c>
+      <c r="J6" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K6" s="23" t="s">
+      <c r="K6" s="21" t="s">
         <v>332</v>
       </c>
-      <c r="L6" s="23" t="s">
+      <c r="L6" s="21" t="s">
         <v>333</v>
       </c>
-      <c r="M6" s="23" t="s">
+      <c r="M6" s="21" t="s">
         <v>334</v>
       </c>
-      <c r="N6" s="23" t="s">
+      <c r="N6" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="O6" s="38" t="s">
+      <c r="O6" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="P6" s="23">
+      <c r="P6" s="21">
         <v>1</v>
       </c>
-      <c r="Q6" s="23" t="s">
+      <c r="Q6" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="R6" s="23" t="s">
+      <c r="R6" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S6" s="23" t="s">
+      <c r="S6" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="T6" s="31" t="s">
+      <c r="T6" s="29" t="s">
         <v>303</v>
       </c>
-      <c r="U6" s="55" t="s">
+      <c r="U6" s="49" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30">
+      <c r="A7" s="28">
         <v>4</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="30">
         <v>1994</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="28">
         <v>2</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="19">
         <v>0</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="19">
         <v>1</v>
       </c>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7" s="28">
         <v>1200</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="19" t="s">
         <v>321</v>
       </c>
-      <c r="L7" s="21" t="s">
+      <c r="L7" s="19" t="s">
         <v>337</v>
       </c>
-      <c r="M7" s="21" t="s">
+      <c r="M7" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="N7" s="21" t="s">
+      <c r="N7" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O7" s="39" t="s">
+      <c r="O7" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="P7" s="21">
+      <c r="P7" s="19">
         <v>1</v>
       </c>
-      <c r="Q7" s="21" t="s">
+      <c r="Q7" s="19" t="s">
         <v>304</v>
       </c>
-      <c r="R7" s="21" t="s">
+      <c r="R7" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="S7" s="21" t="s">
+      <c r="S7" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="T7" s="32" t="s">
-        <v>214</v>
-      </c>
-      <c r="U7" s="56"/>
+      <c r="T7" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="U7" s="50"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="30">
+      <c r="A8" s="28">
         <v>8</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="29">
         <v>2018</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="28">
         <v>1</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="21">
         <v>1</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="21">
         <v>1</v>
       </c>
-      <c r="H8" s="31" t="s">
+      <c r="H8" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="37">
-        <v>400</v>
-      </c>
-      <c r="J8" s="23" t="s">
+      <c r="I8" s="35">
+        <v>400</v>
+      </c>
+      <c r="J8" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K8" s="23">
+      <c r="K8" s="21">
         <v>8</v>
       </c>
-      <c r="L8" s="23">
+      <c r="L8" s="21">
         <v>34</v>
       </c>
-      <c r="M8" s="23">
+      <c r="M8" s="21">
         <v>64</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="N8" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O8" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="P8" s="21">
+      <c r="O8" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q8" s="23" t="s">
+      <c r="Q8" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="R8" s="23" t="s">
+      <c r="R8" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S8" s="23" t="s">
+      <c r="S8" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="T8" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="U8" s="55"/>
+      <c r="T8" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="U8" s="49"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="30">
+      <c r="A9" s="28">
         <v>9</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="29">
         <v>2004</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="28">
         <v>1</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="21">
         <v>1</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="21">
         <v>1</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="H9" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="37">
-        <v>400</v>
-      </c>
-      <c r="J9" s="23" t="s">
+      <c r="I9" s="35">
+        <v>400</v>
+      </c>
+      <c r="J9" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K9" s="23">
+      <c r="K9" s="21">
         <v>20</v>
       </c>
-      <c r="L9" s="23" t="s">
+      <c r="L9" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="23" t="s">
+      <c r="M9" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="N9" s="21" t="s">
+      <c r="N9" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O9" s="38" t="s">
+      <c r="O9" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="P9" s="23">
+      <c r="P9" s="21">
         <v>1</v>
       </c>
-      <c r="Q9" s="23" t="s">
+      <c r="Q9" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="R9" s="23" t="s">
+      <c r="R9" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="S9" s="23" t="s">
+      <c r="S9" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="T9" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="U9" s="55"/>
+      <c r="T9" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="U9" s="49"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="30">
+      <c r="A10" s="28">
         <v>10</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="29">
         <v>2018</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="28">
         <v>1</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="21">
         <v>1</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="21">
         <v>1</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="37">
-        <v>400</v>
-      </c>
-      <c r="J10" s="23" t="s">
+      <c r="I10" s="35">
+        <v>400</v>
+      </c>
+      <c r="J10" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K10" s="23">
+      <c r="K10" s="21">
         <v>7</v>
       </c>
-      <c r="L10" s="23" t="s">
+      <c r="L10" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="M10" s="23" t="s">
+      <c r="M10" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="N10" s="21" t="s">
+      <c r="N10" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O10" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="P10" s="38" t="s">
+      <c r="O10" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="P10" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="Q10" s="23" t="s">
+      <c r="Q10" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="R10" s="23" t="s">
+      <c r="R10" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S10" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="T10" s="31" t="s">
+      <c r="S10" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="T10" s="29" t="s">
         <v>310</v>
       </c>
-      <c r="U10" s="55"/>
+      <c r="U10" s="49"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="30">
+      <c r="A11" s="28">
         <v>11</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="29">
         <v>2009</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="28">
         <v>3</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="21">
         <v>1</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="21">
         <v>1</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="37">
-        <v>400</v>
-      </c>
-      <c r="J11" s="23" t="s">
+      <c r="I11" s="35">
+        <v>400</v>
+      </c>
+      <c r="J11" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K11" s="23">
+      <c r="K11" s="21">
         <v>8</v>
       </c>
-      <c r="L11" s="23">
+      <c r="L11" s="21">
         <v>31</v>
       </c>
-      <c r="M11" s="23">
+      <c r="M11" s="21">
         <v>73</v>
       </c>
-      <c r="N11" s="21" t="s">
+      <c r="N11" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O11" s="38" t="s">
+      <c r="O11" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="P11" s="23">
+      <c r="P11" s="21">
         <v>1</v>
       </c>
-      <c r="Q11" s="23" t="s">
+      <c r="Q11" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="R11" s="23" t="s">
+      <c r="R11" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S11" s="23" t="s">
+      <c r="S11" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="T11" s="31" t="s">
+      <c r="T11" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="U11" s="55" t="s">
+      <c r="U11" s="49" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="30">
+      <c r="A12" s="28">
         <v>12</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="29">
         <v>1990</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="28">
         <v>1</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="21">
         <v>0</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="21">
         <v>1</v>
       </c>
-      <c r="H12" s="31" t="s">
+      <c r="H12" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="37">
+      <c r="I12" s="35">
         <v>200</v>
       </c>
-      <c r="J12" s="23" t="s">
+      <c r="J12" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K12" s="23">
+      <c r="K12" s="21">
         <v>1</v>
       </c>
-      <c r="L12" s="23" t="s">
+      <c r="L12" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="M12" s="23" t="s">
+      <c r="M12" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="N12" s="21" t="s">
+      <c r="N12" s="19" t="s">
         <v>347</v>
       </c>
-      <c r="O12" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="P12" s="23">
+      <c r="O12" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="P12" s="21">
         <v>0</v>
       </c>
-      <c r="Q12" s="23" t="s">
+      <c r="Q12" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="R12" s="23" t="s">
+      <c r="R12" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S12" s="23" t="s">
+      <c r="S12" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="T12" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="U12" s="55"/>
+      <c r="T12" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="U12" s="49"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="30">
+      <c r="A13" s="28">
         <v>21</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="D13" s="31">
+      <c r="D13" s="29">
         <v>1992</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="28">
         <v>1</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="21">
         <v>0</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="21">
         <v>1</v>
       </c>
-      <c r="H13" s="31" t="s">
+      <c r="H13" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="37">
+      <c r="I13" s="35">
         <v>998.0625</v>
       </c>
-      <c r="J13" s="23" t="s">
+      <c r="J13" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K13" s="23">
+      <c r="K13" s="21">
         <v>8</v>
       </c>
-      <c r="L13" s="23">
+      <c r="L13" s="21">
         <v>45</v>
       </c>
-      <c r="M13" s="23">
+      <c r="M13" s="21">
         <v>67</v>
       </c>
-      <c r="N13" s="21" t="s">
+      <c r="N13" s="19" t="s">
         <v>347</v>
       </c>
-      <c r="O13" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="P13" s="23">
+      <c r="O13" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="P13" s="21">
         <v>0.75</v>
       </c>
-      <c r="Q13" s="23" t="s">
+      <c r="Q13" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="R13" s="23" t="s">
+      <c r="R13" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S13" s="23" t="s">
+      <c r="S13" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="T13" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="U13" s="55"/>
+      <c r="T13" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="U13" s="49"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="30">
+      <c r="A14" s="28">
         <v>22</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="29">
         <v>1997</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="28">
         <v>1</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="21">
         <v>0</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="21">
         <v>1</v>
       </c>
-      <c r="H14" s="31" t="s">
+      <c r="H14" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="37">
+      <c r="I14" s="35">
         <v>393</v>
       </c>
-      <c r="J14" s="23" t="s">
+      <c r="J14" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K14" s="23">
+      <c r="K14" s="21">
         <v>8</v>
       </c>
-      <c r="L14" s="23">
+      <c r="L14" s="21">
         <v>7</v>
       </c>
-      <c r="M14" s="23">
+      <c r="M14" s="21">
         <v>26.2</v>
       </c>
-      <c r="N14" s="21" t="s">
+      <c r="N14" s="19" t="s">
         <v>347</v>
       </c>
-      <c r="O14" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="P14" s="23">
+      <c r="O14" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="P14" s="21">
         <f>5/8</f>
         <v>0.625</v>
       </c>
-      <c r="Q14" s="23" t="s">
+      <c r="Q14" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="R14" s="23" t="s">
+      <c r="R14" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="S14" s="23" t="s">
+      <c r="S14" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="T14" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="U14" s="55" t="s">
+      <c r="T14" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="U14" s="49" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="30">
+      <c r="A15" s="28">
         <v>23</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="D15" s="31">
+      <c r="D15" s="29">
         <v>2002</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E15" s="28">
         <v>1</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="21">
         <v>1</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="21">
         <v>1</v>
       </c>
-      <c r="H15" s="31" t="s">
+      <c r="H15" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="37">
-        <v>400</v>
-      </c>
-      <c r="J15" s="23" t="s">
+      <c r="I15" s="35">
+        <v>400</v>
+      </c>
+      <c r="J15" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K15" s="23">
+      <c r="K15" s="21">
         <v>1</v>
       </c>
-      <c r="L15" s="23" t="s">
+      <c r="L15" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="M15" s="23" t="s">
+      <c r="M15" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="N15" s="21" t="s">
+      <c r="N15" s="19" t="s">
         <v>347</v>
       </c>
-      <c r="O15" s="38" t="s">
+      <c r="O15" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="P15" s="23" t="s">
+      <c r="P15" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="Q15" s="23" t="s">
+      <c r="Q15" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="R15" s="23" t="s">
+      <c r="R15" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="S15" s="23" t="s">
+      <c r="S15" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="T15" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="U15" s="55"/>
+      <c r="T15" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="U15" s="49"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="30">
+      <c r="A16" s="28">
         <v>26</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="29">
         <v>1988</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="28">
         <v>2</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="21">
         <v>0</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="21">
         <v>1</v>
       </c>
-      <c r="H16" s="31" t="s">
+      <c r="H16" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="37">
-        <v>400</v>
-      </c>
-      <c r="J16" s="23" t="s">
+      <c r="I16" s="35">
+        <v>400</v>
+      </c>
+      <c r="J16" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K16" s="23">
+      <c r="K16" s="21">
         <v>6</v>
       </c>
-      <c r="L16" s="23">
+      <c r="L16" s="21">
         <v>43</v>
       </c>
-      <c r="M16" s="23">
+      <c r="M16" s="21">
         <v>70.8</v>
       </c>
-      <c r="N16" s="21" t="s">
+      <c r="N16" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O16" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="P16" s="23">
+      <c r="O16" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="P16" s="21">
         <f>5/6</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q16" s="23" t="s">
+      <c r="Q16" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="R16" s="23" t="s">
+      <c r="R16" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S16" s="23" t="s">
+      <c r="S16" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="T16" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="U16" s="55"/>
+      <c r="T16" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="U16" s="49"/>
     </row>
     <row r="17" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16380" x14ac:dyDescent="0.25">
-      <c r="A17" s="30">
+      <c r="A17" s="28">
         <v>27</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D17" s="31">
+      <c r="D17" s="29">
         <v>2010</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="28">
         <v>2</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="21">
         <v>0</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="21">
         <v>1</v>
       </c>
-      <c r="H17" s="31" t="s">
+      <c r="H17" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="37">
-        <v>400</v>
-      </c>
-      <c r="J17" s="23" t="s">
+      <c r="I17" s="35">
+        <v>400</v>
+      </c>
+      <c r="J17" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K17" s="23">
+      <c r="K17" s="21">
         <v>9</v>
       </c>
-      <c r="L17" s="23">
+      <c r="L17" s="21">
         <v>26</v>
       </c>
-      <c r="M17" s="23">
+      <c r="M17" s="21">
         <v>64.2</v>
       </c>
-      <c r="N17" s="21" t="s">
+      <c r="N17" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O17" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="P17" s="23">
+      <c r="O17" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="P17" s="21">
         <f>4/9</f>
         <v>0.44444444444444442</v>
       </c>
-      <c r="Q17" s="23" t="s">
+      <c r="Q17" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="R17" s="23" t="s">
+      <c r="R17" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S17" s="23" t="s">
+      <c r="S17" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="T17" s="31" t="s">
+      <c r="T17" s="29" t="s">
         <v>306</v>
       </c>
-      <c r="U17" s="55"/>
+      <c r="U17" s="49"/>
     </row>
     <row r="18" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16380" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30">
+      <c r="A18" s="28">
         <v>29</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="30">
         <v>1986</v>
       </c>
-      <c r="E18" s="30">
-        <v>3</v>
-      </c>
-      <c r="F18" s="21">
+      <c r="E18" s="28">
+        <v>8</v>
+      </c>
+      <c r="F18" s="19">
         <v>0</v>
       </c>
-      <c r="G18" s="21">
+      <c r="G18" s="19">
         <v>1</v>
       </c>
-      <c r="H18" s="32" t="s">
+      <c r="H18" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="30">
-        <v>400</v>
-      </c>
-      <c r="J18" s="21" t="s">
+      <c r="I18" s="28">
+        <v>400</v>
+      </c>
+      <c r="J18" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="K18" s="40" t="s">
+      <c r="K18" s="38" t="s">
         <v>365</v>
       </c>
-      <c r="L18" s="21" t="s">
+      <c r="L18" s="19" t="s">
         <v>366</v>
       </c>
-      <c r="M18" s="21" t="s">
+      <c r="M18" s="19" t="s">
         <v>367</v>
       </c>
-      <c r="N18" s="21" t="s">
+      <c r="N18" s="19" t="s">
         <v>347</v>
       </c>
-      <c r="O18" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="P18" s="21" t="s">
+      <c r="O18" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="P18" s="19" t="s">
         <v>314</v>
       </c>
-      <c r="Q18" s="23" t="s">
+      <c r="Q18" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="R18" s="21" t="s">
+      <c r="R18" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="S18" s="21" t="s">
+      <c r="S18" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="T18" s="32" t="s">
-        <v>214</v>
-      </c>
-      <c r="U18" s="56" t="s">
+      <c r="T18" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="U18" s="50" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16380" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30">
+      <c r="A19" s="28">
         <v>32</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="30">
         <v>2003</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="28">
         <v>1</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="19">
         <v>0</v>
       </c>
-      <c r="G19" s="21">
+      <c r="G19" s="19">
         <v>1</v>
       </c>
-      <c r="H19" s="32" t="s">
+      <c r="H19" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I19" s="30">
+      <c r="I19" s="28">
         <v>800</v>
       </c>
-      <c r="J19" s="21" t="s">
+      <c r="J19" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="K19" s="21">
+      <c r="K19" s="19">
         <v>12</v>
       </c>
-      <c r="L19" s="21">
+      <c r="L19" s="19">
         <v>30</v>
       </c>
-      <c r="M19" s="21">
+      <c r="M19" s="19">
         <v>67.7</v>
       </c>
-      <c r="N19" s="21" t="s">
+      <c r="N19" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O19" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="P19" s="21">
+      <c r="O19" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="P19" s="19">
         <f>8/12</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="Q19" s="21" t="s">
+      <c r="Q19" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="R19" s="21" t="s">
+      <c r="R19" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="S19" s="21" t="s">
+      <c r="S19" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="T19" s="32" t="s">
-        <v>214</v>
-      </c>
-      <c r="U19" s="56"/>
+      <c r="T19" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="U19" s="50"/>
     </row>
     <row r="20" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16380" x14ac:dyDescent="0.25">
-      <c r="A20" s="30">
+      <c r="A20" s="28">
         <v>33</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="D20" s="31">
+      <c r="D20" s="29">
         <v>2002</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="28">
         <v>3</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F20" s="21">
         <v>0</v>
       </c>
-      <c r="G20" s="23">
+      <c r="G20" s="21">
         <v>1</v>
       </c>
-      <c r="H20" s="31" t="s">
+      <c r="H20" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I20" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="J20" s="23" t="s">
+      <c r="I20" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K20" s="21">
+      <c r="K20" s="19">
         <v>10</v>
       </c>
-      <c r="L20" s="21">
+      <c r="L20" s="19">
         <v>33</v>
       </c>
-      <c r="M20" s="21">
+      <c r="M20" s="19">
         <v>64</v>
       </c>
-      <c r="N20" s="21" t="s">
+      <c r="N20" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O20" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="P20" s="23">
+      <c r="O20" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="P20" s="21">
         <f>6/10</f>
         <v>0.6</v>
       </c>
-      <c r="Q20" s="23" t="s">
+      <c r="Q20" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="R20" s="23" t="s">
+      <c r="R20" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S20" s="23" t="s">
+      <c r="S20" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="T20" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="U20" s="55" t="s">
+      <c r="T20" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="U20" s="49" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16380" x14ac:dyDescent="0.25">
-      <c r="A21" s="30">
+      <c r="A21" s="28">
         <v>34</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="29">
         <v>2006</v>
       </c>
-      <c r="E21" s="30">
+      <c r="E21" s="28">
         <v>2</v>
       </c>
-      <c r="F21" s="23">
+      <c r="F21" s="21">
         <v>0</v>
       </c>
-      <c r="G21" s="23">
+      <c r="G21" s="21">
         <v>1</v>
       </c>
-      <c r="H21" s="31" t="s">
+      <c r="H21" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I21" s="37">
-        <v>400</v>
-      </c>
-      <c r="J21" s="23" t="s">
+      <c r="I21" s="35">
+        <v>400</v>
+      </c>
+      <c r="J21" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K21" s="21">
+      <c r="K21" s="19">
         <v>23</v>
       </c>
-      <c r="L21" s="21">
+      <c r="L21" s="19">
         <v>21</v>
       </c>
-      <c r="M21" s="21">
+      <c r="M21" s="19">
         <v>53.1</v>
       </c>
-      <c r="N21" s="21" t="s">
+      <c r="N21" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O21" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="P21" s="23">
+      <c r="O21" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="P21" s="21">
         <f>12/23</f>
         <v>0.52173913043478259</v>
       </c>
-      <c r="Q21" s="23" t="s">
+      <c r="Q21" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="R21" s="23" t="s">
+      <c r="R21" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S21" s="23" t="s">
+      <c r="S21" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="T21" s="31" t="s">
+      <c r="T21" s="29" t="s">
         <v>307</v>
       </c>
-      <c r="U21" s="55" t="s">
+      <c r="U21" s="49" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16380" x14ac:dyDescent="0.25">
-      <c r="A22" s="30">
+      <c r="A22" s="28">
         <v>35</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D22" s="31">
+      <c r="D22" s="29">
         <v>2002</v>
       </c>
-      <c r="E22" s="30">
+      <c r="E22" s="28">
         <v>4</v>
       </c>
-      <c r="F22" s="23">
+      <c r="F22" s="21">
         <v>0</v>
       </c>
-      <c r="G22" s="23">
+      <c r="G22" s="21">
         <v>1</v>
       </c>
-      <c r="H22" s="31" t="s">
+      <c r="H22" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="I22" s="37">
+      <c r="I22" s="35">
         <v>690</v>
       </c>
-      <c r="J22" s="23" t="s">
+      <c r="J22" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K22" s="21">
+      <c r="K22" s="19">
         <v>6</v>
       </c>
-      <c r="L22" s="21">
+      <c r="L22" s="19">
         <v>20</v>
       </c>
-      <c r="M22" s="21">
+      <c r="M22" s="19">
         <v>69</v>
       </c>
-      <c r="N22" s="21" t="s">
+      <c r="N22" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O22" s="38" t="s">
+      <c r="O22" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="P22" s="23">
+      <c r="P22" s="21">
         <v>1</v>
       </c>
-      <c r="Q22" s="23" t="s">
+      <c r="Q22" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="R22" s="23" t="s">
+      <c r="R22" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S22" s="23" t="s">
+      <c r="S22" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="T22" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="U22" s="55"/>
+      <c r="T22" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="U22" s="49"/>
     </row>
     <row r="23" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16380" x14ac:dyDescent="0.25">
-      <c r="A23" s="30">
+      <c r="A23" s="28">
         <v>36</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="D23" s="31">
+      <c r="D23" s="29">
         <v>1993</v>
       </c>
-      <c r="E23" s="30">
+      <c r="E23" s="28">
         <v>1</v>
       </c>
-      <c r="F23" s="23">
+      <c r="F23" s="21">
         <v>0</v>
       </c>
-      <c r="G23" s="23">
+      <c r="G23" s="21">
         <v>1</v>
       </c>
-      <c r="H23" s="31" t="s">
+      <c r="H23" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="J23" s="23" t="s">
+      <c r="I23" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K23" s="21">
+      <c r="K23" s="19">
         <v>5</v>
       </c>
-      <c r="L23" s="21">
+      <c r="L23" s="19">
         <v>9</v>
       </c>
-      <c r="M23" s="21">
+      <c r="M23" s="19">
         <v>26.8</v>
       </c>
-      <c r="N23" s="21" t="s">
+      <c r="N23" s="19" t="s">
         <v>347</v>
       </c>
-      <c r="O23" s="38" t="s">
+      <c r="O23" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="P23" s="23">
+      <c r="P23" s="21">
         <v>1</v>
       </c>
-      <c r="Q23" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="R23" s="23" t="s">
+      <c r="Q23" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="R23" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="S23" s="23" t="s">
+      <c r="S23" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="T23" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="U23" s="55"/>
+      <c r="T23" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="U23" s="49"/>
     </row>
     <row r="24" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16380" x14ac:dyDescent="0.25">
-      <c r="A24" s="30">
+      <c r="A24" s="28">
         <v>38</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="D24" s="31">
+      <c r="D24" s="29">
         <v>2004</v>
       </c>
-      <c r="E24" s="30">
+      <c r="E24" s="28">
         <v>2</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="21">
         <v>1</v>
       </c>
-      <c r="G24" s="23">
+      <c r="G24" s="21">
         <v>1</v>
       </c>
-      <c r="H24" s="31" t="s">
+      <c r="H24" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I24" s="37">
-        <v>400</v>
-      </c>
-      <c r="J24" s="23" t="s">
+      <c r="I24" s="35">
+        <v>400</v>
+      </c>
+      <c r="J24" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K24" s="41" t="s">
+      <c r="K24" s="39" t="s">
         <v>390</v>
       </c>
-      <c r="L24" s="23" t="s">
+      <c r="L24" s="21" t="s">
         <v>391</v>
       </c>
-      <c r="M24" s="23" t="s">
+      <c r="M24" s="21" t="s">
         <v>392</v>
       </c>
-      <c r="N24" s="21" t="s">
+      <c r="N24" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O24" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="P24" s="23">
+      <c r="O24" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="P24" s="21">
         <f>14/20</f>
         <v>0.7</v>
       </c>
-      <c r="Q24" s="23" t="s">
+      <c r="Q24" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="R24" s="23" t="s">
+      <c r="R24" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="S24" s="23" t="s">
+      <c r="S24" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="T24" s="31" t="s">
+      <c r="T24" s="29" t="s">
         <v>306</v>
       </c>
-      <c r="U24" s="55" t="s">
+      <c r="U24" s="49" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="25" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16380" x14ac:dyDescent="0.25">
-      <c r="A25" s="30">
+      <c r="A25" s="28">
         <v>40</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="D25" s="31">
+      <c r="D25" s="29">
         <v>2004</v>
       </c>
-      <c r="E25" s="30">
+      <c r="E25" s="28">
         <v>1</v>
       </c>
-      <c r="F25" s="23">
+      <c r="F25" s="21">
         <v>0</v>
       </c>
-      <c r="G25" s="23">
+      <c r="G25" s="21">
         <v>1</v>
       </c>
-      <c r="H25" s="31" t="s">
+      <c r="H25" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="I25" s="37">
-        <v>400</v>
-      </c>
-      <c r="J25" s="23" t="s">
+      <c r="I25" s="35">
+        <v>400</v>
+      </c>
+      <c r="J25" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K25" s="21">
+      <c r="K25" s="19">
         <v>10</v>
       </c>
-      <c r="L25" s="21">
+      <c r="L25" s="19">
         <v>29</v>
       </c>
-      <c r="M25" s="21">
+      <c r="M25" s="19">
         <v>83</v>
       </c>
-      <c r="N25" s="21" t="s">
+      <c r="N25" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O25" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="P25" s="23">
+      <c r="O25" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="P25" s="21">
         <f>4/10</f>
         <v>0.4</v>
       </c>
-      <c r="Q25" s="23" t="s">
+      <c r="Q25" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="R25" s="23" t="s">
+      <c r="R25" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S25" s="23" t="s">
+      <c r="S25" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="T25" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="U25" s="55"/>
+      <c r="T25" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="U25" s="49"/>
     </row>
     <row r="26" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16380" x14ac:dyDescent="0.25">
-      <c r="A26" s="30">
+      <c r="A26" s="28">
         <v>42</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="D26" s="31">
+      <c r="D26" s="29">
         <v>2000</v>
       </c>
-      <c r="E26" s="30">
+      <c r="E26" s="28">
         <v>5</v>
       </c>
-      <c r="F26" s="23">
+      <c r="F26" s="21">
         <v>0</v>
       </c>
-      <c r="G26" s="23">
+      <c r="G26" s="21">
         <v>1</v>
       </c>
-      <c r="H26" s="31" t="s">
+      <c r="H26" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="I26" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="J26" s="23" t="s">
+      <c r="I26" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K26" s="21">
+      <c r="K26" s="19">
         <v>6</v>
       </c>
-      <c r="L26" s="21">
+      <c r="L26" s="19">
         <v>20</v>
       </c>
-      <c r="M26" s="21">
+      <c r="M26" s="19">
         <v>77</v>
       </c>
-      <c r="N26" s="21" t="s">
+      <c r="N26" s="19" t="s">
         <v>398</v>
       </c>
-      <c r="O26" s="38" t="s">
+      <c r="O26" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="P26" s="23">
+      <c r="P26" s="21">
         <v>1</v>
       </c>
-      <c r="Q26" s="23" t="s">
+      <c r="Q26" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="R26" s="23" t="s">
+      <c r="R26" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S26" s="23" t="s">
+      <c r="S26" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="T26" s="31" t="s">
+      <c r="T26" s="29" t="s">
         <v>440</v>
       </c>
-      <c r="U26" s="55"/>
+      <c r="U26" s="49"/>
     </row>
     <row r="27" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16380" x14ac:dyDescent="0.25">
-      <c r="A27" s="30">
+      <c r="A27" s="28">
         <v>43</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="D27" s="31">
+      <c r="D27" s="29">
         <v>2019</v>
       </c>
-      <c r="E27" s="30">
+      <c r="E27" s="28">
         <v>1</v>
       </c>
-      <c r="F27" s="23">
+      <c r="F27" s="21">
         <v>1</v>
       </c>
-      <c r="G27" s="23">
+      <c r="G27" s="21">
         <v>1</v>
       </c>
-      <c r="H27" s="31" t="s">
+      <c r="H27" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I27" s="37">
-        <v>400</v>
-      </c>
-      <c r="J27" s="23" t="s">
+      <c r="I27" s="35">
+        <v>400</v>
+      </c>
+      <c r="J27" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K27" s="21">
+      <c r="K27" s="19">
         <v>10</v>
       </c>
-      <c r="L27" s="21">
+      <c r="L27" s="19">
         <v>16</v>
       </c>
-      <c r="M27" s="21">
+      <c r="M27" s="19">
         <v>55</v>
       </c>
-      <c r="N27" s="21" t="s">
+      <c r="N27" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O27" s="38" t="s">
+      <c r="O27" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="P27" s="23">
+      <c r="P27" s="21">
         <v>1</v>
       </c>
-      <c r="Q27" s="23" t="s">
+      <c r="Q27" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="R27" s="23" t="s">
+      <c r="R27" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="S27" s="23" t="s">
+      <c r="S27" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="T27" s="31" t="s">
+      <c r="T27" s="29" t="s">
         <v>272</v>
       </c>
-      <c r="U27" s="55"/>
+      <c r="U27" s="49"/>
     </row>
     <row r="28" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16380" x14ac:dyDescent="0.25">
-      <c r="A28" s="30">
+      <c r="A28" s="28">
         <v>44</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="D28" s="31">
+      <c r="D28" s="29">
         <v>2002</v>
       </c>
-      <c r="E28" s="30">
+      <c r="E28" s="28">
         <v>2</v>
       </c>
-      <c r="F28" s="23">
+      <c r="F28" s="21">
         <v>1</v>
       </c>
-      <c r="G28" s="23">
+      <c r="G28" s="21">
         <v>1</v>
       </c>
-      <c r="H28" s="31" t="s">
+      <c r="H28" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I28" s="37">
-        <v>400</v>
-      </c>
-      <c r="J28" s="23" t="s">
+      <c r="I28" s="35">
+        <v>400</v>
+      </c>
+      <c r="J28" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K28" s="21">
+      <c r="K28" s="19">
         <v>14</v>
       </c>
-      <c r="L28" s="21">
+      <c r="L28" s="19">
         <v>35</v>
       </c>
-      <c r="M28" s="21">
+      <c r="M28" s="19">
         <v>36.5</v>
       </c>
-      <c r="N28" s="21" t="s">
+      <c r="N28" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O28" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="P28" s="23">
+      <c r="O28" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="P28" s="21">
         <f>34/42</f>
         <v>0.80952380952380953</v>
       </c>
-      <c r="Q28" s="23" t="s">
+      <c r="Q28" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="R28" s="23" t="s">
+      <c r="R28" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S28" s="23" t="s">
+      <c r="S28" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="T28" s="31" t="s">
+      <c r="T28" s="29" t="s">
         <v>308</v>
       </c>
-      <c r="U28" s="55" t="s">
+      <c r="U28" s="49" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="29" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16380" x14ac:dyDescent="0.25">
-      <c r="A29" s="30">
+      <c r="A29" s="28">
         <v>48</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="D29" s="31">
+      <c r="D29" s="29">
         <v>2016</v>
       </c>
-      <c r="E29" s="35">
+      <c r="E29" s="33">
         <v>2</v>
       </c>
-      <c r="F29" s="23">
+      <c r="F29" s="21">
         <v>0</v>
       </c>
-      <c r="G29" s="36">
+      <c r="G29" s="34">
         <v>1</v>
       </c>
-      <c r="H29" s="31" t="s">
+      <c r="H29" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I29" s="37">
-        <v>400</v>
-      </c>
-      <c r="J29" s="23" t="s">
+      <c r="I29" s="35">
+        <v>400</v>
+      </c>
+      <c r="J29" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K29" s="41" t="s">
+      <c r="K29" s="39" t="s">
         <v>409</v>
       </c>
-      <c r="L29" s="23" t="s">
+      <c r="L29" s="21" t="s">
         <v>408</v>
       </c>
-      <c r="M29" s="23" t="s">
+      <c r="M29" s="21" t="s">
         <v>410</v>
       </c>
-      <c r="N29" s="21" t="s">
+      <c r="N29" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O29" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="P29" s="36">
+      <c r="O29" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="P29" s="34">
         <v>0.5</v>
       </c>
-      <c r="Q29" s="23" t="s">
+      <c r="Q29" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="R29" s="23" t="s">
+      <c r="R29" s="21" t="s">
         <v>280</v>
       </c>
-      <c r="S29" s="23" t="s">
+      <c r="S29" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="T29" s="43" t="s">
+      <c r="T29" s="41" t="s">
         <v>309</v>
       </c>
-      <c r="U29" s="55" t="s">
+      <c r="U29" s="49" t="s">
         <v>193</v>
       </c>
       <c r="X29" s="6"/>
@@ -7805,399 +7805,399 @@
       <c r="XEZ29" s="6"/>
     </row>
     <row r="30" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16380" x14ac:dyDescent="0.25">
-      <c r="A30" s="30">
+      <c r="A30" s="28">
         <v>51</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="D30" s="31">
+      <c r="D30" s="29">
         <v>2002</v>
       </c>
-      <c r="E30" s="30">
+      <c r="E30" s="28">
         <v>1</v>
       </c>
-      <c r="F30" s="23">
+      <c r="F30" s="21">
         <v>0</v>
       </c>
-      <c r="G30" s="23">
+      <c r="G30" s="21">
         <v>1</v>
       </c>
-      <c r="H30" s="31" t="s">
+      <c r="H30" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="I30" s="37">
+      <c r="I30" s="35">
         <v>830</v>
       </c>
-      <c r="J30" s="23" t="s">
+      <c r="J30" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K30" s="21">
+      <c r="K30" s="19">
         <v>7</v>
       </c>
-      <c r="L30" s="21">
+      <c r="L30" s="19">
         <v>29</v>
       </c>
-      <c r="M30" s="21">
+      <c r="M30" s="19">
         <v>66.400000000000006</v>
       </c>
-      <c r="N30" s="21" t="s">
+      <c r="N30" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O30" s="38" t="s">
+      <c r="O30" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="P30" s="23">
+      <c r="P30" s="21">
         <v>1</v>
       </c>
-      <c r="Q30" s="23" t="s">
+      <c r="Q30" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="R30" s="23" t="s">
+      <c r="R30" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S30" s="23" t="s">
+      <c r="S30" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="T30" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="U30" s="55"/>
+      <c r="T30" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="U30" s="49"/>
     </row>
     <row r="31" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16380" x14ac:dyDescent="0.25">
-      <c r="A31" s="30">
+      <c r="A31" s="28">
         <v>52</v>
       </c>
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="D31" s="31">
+      <c r="D31" s="29">
         <v>2004</v>
       </c>
-      <c r="E31" s="30">
+      <c r="E31" s="28">
         <v>1</v>
       </c>
-      <c r="F31" s="23">
+      <c r="F31" s="21">
         <v>0</v>
       </c>
-      <c r="G31" s="23">
+      <c r="G31" s="21">
         <v>1</v>
       </c>
-      <c r="H31" s="31" t="s">
+      <c r="H31" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I31" s="37">
+      <c r="I31" s="35">
         <v>600</v>
       </c>
-      <c r="J31" s="23" t="s">
+      <c r="J31" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K31" s="21">
+      <c r="K31" s="19">
         <v>10</v>
       </c>
-      <c r="L31" s="21">
+      <c r="L31" s="19">
         <v>32</v>
       </c>
-      <c r="M31" s="21">
+      <c r="M31" s="19">
         <v>59.8</v>
       </c>
-      <c r="N31" s="21" t="s">
+      <c r="N31" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O31" s="38" t="s">
+      <c r="O31" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="P31" s="23" t="s">
+      <c r="P31" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="Q31" s="23" t="s">
+      <c r="Q31" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="R31" s="23" t="s">
+      <c r="R31" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S31" s="23" t="s">
+      <c r="S31" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="T31" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="U31" s="55"/>
+      <c r="T31" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="U31" s="49"/>
     </row>
     <row r="32" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16380" x14ac:dyDescent="0.25">
-      <c r="A32" s="30">
+      <c r="A32" s="28">
         <v>53</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D32" s="31">
+      <c r="D32" s="29">
         <v>2005</v>
       </c>
-      <c r="E32" s="30">
+      <c r="E32" s="28">
         <v>2</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F32" s="21">
         <v>0</v>
       </c>
-      <c r="G32" s="23">
+      <c r="G32" s="21">
         <v>1</v>
       </c>
-      <c r="H32" s="31" t="s">
+      <c r="H32" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I32" s="37">
+      <c r="I32" s="35">
         <v>800</v>
       </c>
-      <c r="J32" s="23" t="s">
+      <c r="J32" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K32" s="21">
+      <c r="K32" s="19">
         <v>16</v>
       </c>
-      <c r="L32" s="21">
-        <v>25</v>
-      </c>
-      <c r="M32" s="21">
+      <c r="L32" s="19">
+        <v>25</v>
+      </c>
+      <c r="M32" s="19">
         <v>62.9</v>
       </c>
-      <c r="N32" s="21" t="s">
+      <c r="N32" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O32" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="P32" s="23">
+      <c r="O32" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="P32" s="21">
         <f>9/16</f>
         <v>0.5625</v>
       </c>
-      <c r="Q32" s="23" t="s">
+      <c r="Q32" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="R32" s="23" t="s">
+      <c r="R32" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S32" s="23" t="s">
+      <c r="S32" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="T32" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="U32" s="55"/>
+      <c r="T32" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="U32" s="49"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A33" s="30">
+      <c r="A33" s="28">
         <v>58</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="D33" s="31">
+      <c r="D33" s="29">
         <v>2016</v>
       </c>
-      <c r="E33" s="30">
+      <c r="E33" s="28">
         <v>1</v>
       </c>
-      <c r="F33" s="23">
+      <c r="F33" s="21">
         <v>1</v>
       </c>
-      <c r="G33" s="23">
+      <c r="G33" s="21">
         <v>1</v>
       </c>
-      <c r="H33" s="31" t="s">
+      <c r="H33" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I33" s="37">
-        <v>400</v>
-      </c>
-      <c r="J33" s="23" t="s">
+      <c r="I33" s="35">
+        <v>400</v>
+      </c>
+      <c r="J33" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K33" s="21">
+      <c r="K33" s="19">
         <v>51</v>
       </c>
-      <c r="L33" s="23" t="s">
+      <c r="L33" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="M33" s="23" t="s">
+      <c r="M33" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="N33" s="21" t="s">
+      <c r="N33" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O33" s="38" t="s">
+      <c r="O33" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="P33" s="38" t="s">
+      <c r="P33" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="Q33" s="23" t="s">
+      <c r="Q33" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="R33" s="23" t="s">
+      <c r="R33" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S33" s="23" t="s">
+      <c r="S33" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="T33" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="U33" s="55" t="s">
+      <c r="T33" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="U33" s="49" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A34" s="30">
+      <c r="A34" s="28">
         <v>60</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="D34" s="31">
+      <c r="D34" s="29">
         <v>1991</v>
       </c>
-      <c r="E34" s="30">
+      <c r="E34" s="28">
         <v>1</v>
       </c>
-      <c r="F34" s="23">
+      <c r="F34" s="21">
         <v>0</v>
       </c>
-      <c r="G34" s="23">
+      <c r="G34" s="21">
         <v>1</v>
       </c>
-      <c r="H34" s="31" t="s">
+      <c r="H34" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="I34" s="37">
+      <c r="I34" s="35">
         <v>725</v>
       </c>
-      <c r="J34" s="23" t="s">
+      <c r="J34" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K34" s="21">
+      <c r="K34" s="19">
         <v>4</v>
       </c>
-      <c r="L34" s="23" t="s">
+      <c r="L34" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="M34" s="23">
+      <c r="M34" s="21">
         <v>72</v>
       </c>
-      <c r="N34" s="21" t="s">
+      <c r="N34" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="O34" s="38" t="s">
+      <c r="O34" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="P34" s="23">
+      <c r="P34" s="21">
         <v>1</v>
       </c>
-      <c r="Q34" s="23" t="s">
+      <c r="Q34" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="R34" s="23" t="s">
+      <c r="R34" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="S34" s="23" t="s">
+      <c r="S34" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="T34" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="U34" s="55"/>
+      <c r="T34" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="U34" s="49"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A35" s="33">
+      <c r="A35" s="31">
         <v>62</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="C35" s="26" t="s">
+      <c r="C35" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="D35" s="34">
+      <c r="D35" s="32">
         <v>2019</v>
       </c>
-      <c r="E35" s="33">
+      <c r="E35" s="31">
         <v>2</v>
       </c>
-      <c r="F35" s="27">
+      <c r="F35" s="25">
         <v>1</v>
       </c>
-      <c r="G35" s="26">
+      <c r="G35" s="24">
         <v>1</v>
       </c>
-      <c r="H35" s="34" t="s">
+      <c r="H35" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="I35" s="44">
-        <v>400</v>
-      </c>
-      <c r="J35" s="27" t="s">
+      <c r="I35" s="42">
+        <v>400</v>
+      </c>
+      <c r="J35" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="K35" s="27" t="s">
+      <c r="K35" s="25" t="s">
         <v>425</v>
       </c>
-      <c r="L35" s="27" t="s">
+      <c r="L35" s="25" t="s">
         <v>426</v>
       </c>
-      <c r="M35" s="27" t="s">
+      <c r="M35" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="N35" s="26" t="s">
+      <c r="N35" s="24" t="s">
         <v>329</v>
       </c>
-      <c r="O35" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="P35" s="27" t="s">
+      <c r="O35" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="P35" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="Q35" s="27" t="s">
+      <c r="Q35" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="R35" s="27" t="s">
+      <c r="R35" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="S35" s="27" t="s">
+      <c r="S35" s="25" t="s">
         <v>251</v>
       </c>
-      <c r="T35" s="34" t="s">
+      <c r="T35" s="32" t="s">
         <v>310</v>
       </c>
-      <c r="U35" s="57" t="s">
+      <c r="U35" s="51" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D36" s="53" t="s">
+      <c r="D36" s="47" t="s">
         <v>446</v>
       </c>
-      <c r="E36" s="54">
+      <c r="E36" s="48">
         <f>SUM(E5:E35)</f>
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:23" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A37" s="18"/>
+      <c r="A37" s="16"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -8227,18 +8227,18 @@
       <c r="C38" s="15"/>
       <c r="D38" s="15"/>
       <c r="E38" s="15"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="16"/>
-      <c r="K38" s="16"/>
-      <c r="L38" s="16"/>
-      <c r="M38" s="16"/>
-      <c r="N38" s="16"/>
-      <c r="O38" s="17"/>
-      <c r="P38" s="17"/>
-      <c r="Q38" s="17"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="58"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="57"/>
+      <c r="K38" s="57"/>
+      <c r="L38" s="57"/>
+      <c r="M38" s="57"/>
+      <c r="N38" s="57"/>
+      <c r="O38" s="58"/>
+      <c r="P38" s="58"/>
+      <c r="Q38" s="58"/>
       <c r="R38" s="15"/>
       <c r="S38" s="15"/>
       <c r="T38" s="15"/>
@@ -8284,27 +8284,27 @@
     <row r="49" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="50" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="51" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="19"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="19"/>
-      <c r="I51" s="19"/>
-      <c r="J51" s="19"/>
-      <c r="K51" s="19"/>
-      <c r="L51" s="19"/>
-      <c r="M51" s="19"/>
-      <c r="N51" s="19"/>
-      <c r="O51" s="19"/>
-      <c r="P51" s="19"/>
-      <c r="Q51" s="19"/>
-      <c r="R51" s="19"/>
-      <c r="S51" s="19"/>
-      <c r="T51" s="19"/>
-      <c r="U51" s="19"/>
+      <c r="A51" s="17"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="17"/>
+      <c r="J51" s="17"/>
+      <c r="K51" s="17"/>
+      <c r="L51" s="17"/>
+      <c r="M51" s="17"/>
+      <c r="N51" s="17"/>
+      <c r="O51" s="17"/>
+      <c r="P51" s="17"/>
+      <c r="Q51" s="17"/>
+      <c r="R51" s="17"/>
+      <c r="S51" s="17"/>
+      <c r="T51" s="17"/>
+      <c r="U51" s="17"/>
     </row>
     <row r="52" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>